<commit_message>
logs updates and expiration update as well.
</commit_message>
<xml_diff>
--- a/logs/otp_logs.xlsx
+++ b/logs/otp_logs.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -584,9 +584,93 @@
         <v>901258</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>2025-07-31T04:59:12.791Z</v>
+      </c>
+      <c r="B14" t="str">
+        <v>arpitsin28@gmail.com</v>
+      </c>
+      <c r="C14" t="str">
+        <v>8303884098</v>
+      </c>
+      <c r="D14">
+        <v>582834</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>2025-07-31T05:00:19.028Z</v>
+      </c>
+      <c r="B15" t="str">
+        <v>arpitsin28@gmail.com</v>
+      </c>
+      <c r="C15" t="str">
+        <v>9473733115</v>
+      </c>
+      <c r="D15">
+        <v>947559</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>2025-07-31T05:03:41.962Z</v>
+      </c>
+      <c r="B16" t="str">
+        <v>arpitsin28@gmail.com</v>
+      </c>
+      <c r="C16" t="str">
+        <v>9473733115</v>
+      </c>
+      <c r="D16">
+        <v>140001</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>2025-07-31T05:06:01.226Z</v>
+      </c>
+      <c r="B17" t="str">
+        <v>arpitsin28@gmail.com</v>
+      </c>
+      <c r="C17" t="str">
+        <v>8303884098</v>
+      </c>
+      <c r="D17">
+        <v>442704</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>2025-07-31T05:22:19.516Z</v>
+      </c>
+      <c r="B18" t="str">
+        <v>arpitsin28@gmail.com</v>
+      </c>
+      <c r="C18" t="str">
+        <v>9473733115</v>
+      </c>
+      <c r="D18">
+        <v>269016</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>2025-07-31T05:36:50.240Z</v>
+      </c>
+      <c r="B19" t="str">
+        <v>arpitsin28@gmail.com</v>
+      </c>
+      <c r="C19" t="str">
+        <v>8303884098</v>
+      </c>
+      <c r="D19">
+        <v>656820</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D19"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>